<commit_message>
Added Titles to Excel
</commit_message>
<xml_diff>
--- a/documents/cosineTest.xlsx
+++ b/documents/cosineTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Practia1\PracticaNumero1ProgramacionFuncionalEnHaskell\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82E34548-A294-4D60-AECA-BBE6F01F46F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EA7D83-1BB4-4753-AB21-ACBDFA4F831D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FA1DC8E9-791E-4552-AB03-3DE12A37E227}"/>
   </bookViews>
@@ -19,9 +19,32 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Cos X</t>
+  </si>
+  <si>
+    <t>Degree Of Precision</t>
+  </si>
+  <si>
+    <t>Error Percentage</t>
+  </si>
+  <si>
+    <t>Experimental Cos X</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.00000%"/>
+  </numFmts>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +195,14 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -516,9 +547,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -894,1080 +936,1107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480861B2-0DD1-42A8-BF63-A48AC5515324}">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
         <v>-10</v>
       </c>
-      <c r="B1">
+      <c r="B2" s="1">
         <v>-0.83907149999999997</v>
       </c>
-      <c r="C1">
-        <v>3</v>
-      </c>
-      <c r="D1">
+      <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1">
         <v>-0.48567915</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E2" s="2">
         <v>0.42117070000000001</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
         <v>-9</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="1">
         <v>-0.91113025000000003</v>
       </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
         <v>-0.42052555000000003</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E3" s="2">
         <v>0.53845730000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
         <v>-8</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="1">
         <v>-0.14550003</v>
       </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
         <v>-0.11174798</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E4" s="2">
         <v>0.23197280000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
         <v>-7</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="1">
         <v>0.75390226000000005</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
         <v>0.75408905999999998</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E5" s="2">
         <v>2.4780000000000001E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
         <v>-6</v>
       </c>
-      <c r="B5">
+      <c r="B6" s="1">
         <v>0.96017026999999999</v>
       </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
         <v>0.96017090000000005</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E6" s="2">
         <v>6.9999999999999997E-7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
         <v>-5</v>
       </c>
-      <c r="B6">
+      <c r="B7" s="1">
         <v>0.28366219999999998</v>
       </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
         <v>0.28968322000000002</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E7" s="2">
         <v>2.1225999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
         <v>-4</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="1">
         <v>-0.65364359999999999</v>
       </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7">
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
         <v>-0.47418870000000002</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E8" s="2">
         <v>0.2745455</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="1">
         <v>-3</v>
       </c>
-      <c r="B8">
+      <c r="B9" s="1">
         <v>-0.98999250000000005</v>
       </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
         <v>-0.125</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E9" s="2">
         <v>0.87373639999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="1">
         <v>-2</v>
       </c>
-      <c r="B9">
+      <c r="B10" s="1">
         <v>-0.41614684000000002</v>
       </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9">
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
         <v>-0.33333325000000003</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E10" s="2">
         <v>0.19900090000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="1">
         <v>-1</v>
       </c>
-      <c r="B10">
+      <c r="B11" s="1">
         <v>0.54030230000000001</v>
       </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10">
+      <c r="C11" s="1">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
         <v>0.5416666</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E11" s="2">
         <v>2.5251000000000002E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="1">
         <v>0</v>
       </c>
-      <c r="B11">
+      <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11">
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1">
         <v>1</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E12" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B12">
+      <c r="B13" s="1">
         <v>0.54030230000000001</v>
       </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12">
+      <c r="C13" s="1">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1">
         <v>0.5416666</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E13" s="2">
         <v>2.5251000000000002E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="1">
         <v>2</v>
       </c>
-      <c r="B13">
+      <c r="B14" s="1">
         <v>-0.41614684000000002</v>
       </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="D13">
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1">
         <v>-0.33333325000000003</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E14" s="2">
         <v>0.19900090000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14">
-        <v>3</v>
-      </c>
-      <c r="B14">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="1">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1">
         <v>-0.98999250000000005</v>
       </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
         <v>-0.125</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E15" s="2">
         <v>0.87373639999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="1">
         <v>4</v>
       </c>
-      <c r="B15">
+      <c r="B16" s="1">
         <v>-0.65364359999999999</v>
       </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15">
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
         <v>-0.47418870000000002</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E16" s="2">
         <v>0.2745455</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="1">
         <v>5</v>
       </c>
-      <c r="B16">
+      <c r="B17" s="1">
         <v>0.28366219999999998</v>
       </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16">
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1">
         <v>0.28968322000000002</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E17" s="2">
         <v>2.1225999999999998E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="1">
         <v>6</v>
       </c>
-      <c r="B17">
+      <c r="B18" s="1">
         <v>0.96017026999999999</v>
       </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="D17">
+      <c r="C18" s="1">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1">
         <v>0.96017090000000005</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E18" s="2">
         <v>6.9999999999999997E-7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="1">
         <v>7</v>
       </c>
-      <c r="B18">
+      <c r="B19" s="1">
         <v>0.75390226000000005</v>
       </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18">
+      <c r="C19" s="1">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1">
         <v>0.75408905999999998</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E19" s="2">
         <v>2.4780000000000001E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" s="1">
         <v>8</v>
       </c>
-      <c r="B19">
+      <c r="B20" s="1">
         <v>-0.14550003</v>
       </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-      <c r="D19">
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
         <v>-0.11174798</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E20" s="2">
         <v>0.23197280000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20">
-        <v>9</v>
-      </c>
-      <c r="B20">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="1">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1">
         <v>-0.91113025000000003</v>
       </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="D20">
+      <c r="C21" s="1">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1">
         <v>-0.42052555000000003</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E21" s="2">
         <v>0.53845730000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" s="1">
         <v>10</v>
       </c>
-      <c r="B21">
+      <c r="B22" s="1">
         <v>-0.83907149999999997</v>
       </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21">
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1">
         <v>-0.48567915</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E22" s="2">
         <v>0.42117070000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" s="1">
         <v>-10</v>
       </c>
-      <c r="B22">
+      <c r="B23" s="1">
         <v>-0.83907149999999997</v>
       </c>
-      <c r="C22">
-        <v>9</v>
-      </c>
-      <c r="D22">
+      <c r="C23" s="1">
+        <v>9</v>
+      </c>
+      <c r="D23" s="1">
         <v>-0.83907175000000001</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E23" s="2">
         <v>2.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" s="1">
         <v>-9</v>
       </c>
-      <c r="B23">
+      <c r="B24" s="1">
         <v>-0.91113025000000003</v>
       </c>
-      <c r="C23">
-        <v>9</v>
-      </c>
-      <c r="D23">
+      <c r="C24" s="1">
+        <v>9</v>
+      </c>
+      <c r="D24" s="1">
         <v>-0.91113010000000005</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E24" s="2">
         <v>1.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25" s="1">
         <v>-8</v>
       </c>
-      <c r="B24">
+      <c r="B25" s="1">
         <v>-0.14550003</v>
       </c>
-      <c r="C24">
-        <v>9</v>
-      </c>
-      <c r="D24">
+      <c r="C25" s="1">
+        <v>9</v>
+      </c>
+      <c r="D25" s="1">
         <v>-0.14549993999999999</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E25" s="2">
         <v>5.9999999999999997E-7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" s="1">
         <v>-7</v>
       </c>
-      <c r="B25">
+      <c r="B26" s="1">
         <v>0.75390226000000005</v>
       </c>
-      <c r="C25">
-        <v>9</v>
-      </c>
-      <c r="D25">
+      <c r="C26" s="1">
+        <v>9</v>
+      </c>
+      <c r="D26" s="1">
         <v>0.75390239999999997</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E26" s="2">
         <v>1.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" s="1">
         <v>-6</v>
       </c>
-      <c r="B26">
+      <c r="B27" s="1">
         <v>0.96017026999999999</v>
       </c>
-      <c r="C26">
-        <v>9</v>
-      </c>
-      <c r="D26">
+      <c r="C27" s="1">
+        <v>9</v>
+      </c>
+      <c r="D27" s="1">
         <v>0.96017019999999997</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E27" s="2">
         <v>9.9999999999999995E-8</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" s="1">
         <v>-5</v>
       </c>
-      <c r="B27">
+      <c r="B28" s="1">
         <v>0.28366219999999998</v>
       </c>
-      <c r="C27">
-        <v>9</v>
-      </c>
-      <c r="D27">
+      <c r="C28" s="1">
+        <v>9</v>
+      </c>
+      <c r="D28" s="1">
         <v>0.28366202000000001</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E28" s="2">
         <v>5.9999999999999997E-7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" s="1">
         <v>-4</v>
       </c>
-      <c r="B28">
+      <c r="B29" s="1">
         <v>-0.65364359999999999</v>
       </c>
-      <c r="C28">
-        <v>9</v>
-      </c>
-      <c r="D28">
+      <c r="C29" s="1">
+        <v>9</v>
+      </c>
+      <c r="D29" s="1">
         <v>-0.65364359999999999</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E29" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A30" s="1">
         <v>-3</v>
       </c>
-      <c r="B29">
+      <c r="B30" s="1">
         <v>-0.98999250000000005</v>
       </c>
-      <c r="C29">
-        <v>9</v>
-      </c>
-      <c r="D29">
+      <c r="C30" s="1">
+        <v>9</v>
+      </c>
+      <c r="D30" s="1">
         <v>-0.9899926</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E30" s="2">
         <v>9.9999999999999995E-8</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31" s="1">
         <v>-2</v>
       </c>
-      <c r="B30">
+      <c r="B31" s="1">
         <v>-0.41614684000000002</v>
       </c>
-      <c r="C30">
-        <v>9</v>
-      </c>
-      <c r="D30">
+      <c r="C31" s="1">
+        <v>9</v>
+      </c>
+      <c r="D31" s="1">
         <v>-0.41614676</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E31" s="2">
         <v>1.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A32" s="1">
         <v>-1</v>
       </c>
-      <c r="B31">
+      <c r="B32" s="1">
         <v>0.54030230000000001</v>
       </c>
-      <c r="C31">
-        <v>9</v>
-      </c>
-      <c r="D31">
+      <c r="C32" s="1">
+        <v>9</v>
+      </c>
+      <c r="D32" s="1">
         <v>0.54030230000000001</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E32" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A33" s="1">
         <v>0</v>
       </c>
-      <c r="B32">
+      <c r="B33" s="1">
         <v>1</v>
       </c>
-      <c r="C32">
-        <v>9</v>
-      </c>
-      <c r="D32">
+      <c r="C33" s="1">
+        <v>9</v>
+      </c>
+      <c r="D33" s="1">
         <v>1</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E33" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A34" s="1">
         <v>1</v>
       </c>
-      <c r="B33">
+      <c r="B34" s="1">
         <v>0.54030230000000001</v>
       </c>
-      <c r="C33">
-        <v>9</v>
-      </c>
-      <c r="D33">
+      <c r="C34" s="1">
+        <v>9</v>
+      </c>
+      <c r="D34" s="1">
         <v>0.54030230000000001</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E34" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A35" s="1">
         <v>2</v>
       </c>
-      <c r="B34">
+      <c r="B35" s="1">
         <v>-0.41614684000000002</v>
       </c>
-      <c r="C34">
-        <v>9</v>
-      </c>
-      <c r="D34">
+      <c r="C35" s="1">
+        <v>9</v>
+      </c>
+      <c r="D35" s="1">
         <v>-0.41614676</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E35" s="2">
         <v>1.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35">
-        <v>3</v>
-      </c>
-      <c r="B35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A36" s="1">
+        <v>3</v>
+      </c>
+      <c r="B36" s="1">
         <v>-0.98999250000000005</v>
       </c>
-      <c r="C35">
-        <v>9</v>
-      </c>
-      <c r="D35">
+      <c r="C36" s="1">
+        <v>9</v>
+      </c>
+      <c r="D36" s="1">
         <v>-0.9899926</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E36" s="2">
         <v>9.9999999999999995E-8</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A37" s="1">
         <v>4</v>
       </c>
-      <c r="B36">
+      <c r="B37" s="1">
         <v>-0.65364359999999999</v>
       </c>
-      <c r="C36">
-        <v>9</v>
-      </c>
-      <c r="D36">
+      <c r="C37" s="1">
+        <v>9</v>
+      </c>
+      <c r="D37" s="1">
         <v>-0.65364359999999999</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E37" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A38" s="1">
         <v>5</v>
       </c>
-      <c r="B37">
+      <c r="B38" s="1">
         <v>0.28366219999999998</v>
       </c>
-      <c r="C37">
-        <v>9</v>
-      </c>
-      <c r="D37">
+      <c r="C38" s="1">
+        <v>9</v>
+      </c>
+      <c r="D38" s="1">
         <v>0.28366202000000001</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E38" s="2">
         <v>5.9999999999999997E-7</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A39" s="1">
         <v>6</v>
       </c>
-      <c r="B38">
+      <c r="B39" s="1">
         <v>0.96017026999999999</v>
       </c>
-      <c r="C38">
-        <v>9</v>
-      </c>
-      <c r="D38">
+      <c r="C39" s="1">
+        <v>9</v>
+      </c>
+      <c r="D39" s="1">
         <v>0.96017019999999997</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E39" s="2">
         <v>9.9999999999999995E-8</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A40" s="1">
         <v>7</v>
       </c>
-      <c r="B39">
+      <c r="B40" s="1">
         <v>0.75390226000000005</v>
       </c>
-      <c r="C39">
-        <v>9</v>
-      </c>
-      <c r="D39">
+      <c r="C40" s="1">
+        <v>9</v>
+      </c>
+      <c r="D40" s="1">
         <v>0.75390239999999997</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E40" s="2">
         <v>1.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A41" s="1">
         <v>8</v>
       </c>
-      <c r="B40">
+      <c r="B41" s="1">
         <v>-0.14550003</v>
       </c>
-      <c r="C40">
-        <v>9</v>
-      </c>
-      <c r="D40">
+      <c r="C41" s="1">
+        <v>9</v>
+      </c>
+      <c r="D41" s="1">
         <v>-0.14549993999999999</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E41" s="2">
         <v>5.9999999999999997E-7</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41">
-        <v>9</v>
-      </c>
-      <c r="B41">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A42" s="1">
+        <v>9</v>
+      </c>
+      <c r="B42" s="1">
         <v>-0.91113025000000003</v>
       </c>
-      <c r="C41">
-        <v>9</v>
-      </c>
-      <c r="D41">
+      <c r="C42" s="1">
+        <v>9</v>
+      </c>
+      <c r="D42" s="1">
         <v>-0.91113010000000005</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E42" s="2">
         <v>1.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A43" s="1">
         <v>10</v>
       </c>
-      <c r="B42">
+      <c r="B43" s="1">
         <v>-0.83907149999999997</v>
       </c>
-      <c r="C42">
-        <v>9</v>
-      </c>
-      <c r="D42">
+      <c r="C43" s="1">
+        <v>9</v>
+      </c>
+      <c r="D43" s="1">
         <v>-0.83907175000000001</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E43" s="2">
         <v>2.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A44" s="1">
         <v>-10</v>
       </c>
-      <c r="B43">
+      <c r="B44" s="1">
         <v>-0.83907149999999997</v>
       </c>
-      <c r="C43">
+      <c r="C44" s="1">
         <v>16</v>
       </c>
-      <c r="D43">
+      <c r="D44" s="1">
         <v>-0.83907175000000001</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E44" s="2">
         <v>2.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A45" s="1">
         <v>-9</v>
       </c>
-      <c r="B44">
+      <c r="B45" s="1">
         <v>-0.91113025000000003</v>
       </c>
-      <c r="C44">
+      <c r="C45" s="1">
         <v>16</v>
       </c>
-      <c r="D44">
+      <c r="D45" s="1">
         <v>-0.91113010000000005</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E45" s="2">
         <v>1.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A46" s="1">
         <v>-8</v>
       </c>
-      <c r="B45">
+      <c r="B46" s="1">
         <v>-0.14550003</v>
       </c>
-      <c r="C45">
+      <c r="C46" s="1">
         <v>16</v>
       </c>
-      <c r="D45">
+      <c r="D46" s="1">
         <v>-0.14549993999999999</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E46" s="2">
         <v>5.9999999999999997E-7</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A47" s="1">
         <v>-7</v>
       </c>
-      <c r="B46">
+      <c r="B47" s="1">
         <v>0.75390226000000005</v>
       </c>
-      <c r="C46">
+      <c r="C47" s="1">
         <v>16</v>
       </c>
-      <c r="D46">
+      <c r="D47" s="1">
         <v>0.75390239999999997</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E47" s="2">
         <v>1.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A48" s="1">
         <v>-6</v>
       </c>
-      <c r="B47">
+      <c r="B48" s="1">
         <v>0.96017026999999999</v>
       </c>
-      <c r="C47">
+      <c r="C48" s="1">
         <v>16</v>
       </c>
-      <c r="D47">
+      <c r="D48" s="1">
         <v>0.96017019999999997</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E48" s="2">
         <v>9.9999999999999995E-8</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A49" s="1">
         <v>-5</v>
       </c>
-      <c r="B48">
+      <c r="B49" s="1">
         <v>0.28366219999999998</v>
       </c>
-      <c r="C48">
+      <c r="C49" s="1">
         <v>16</v>
       </c>
-      <c r="D48">
+      <c r="D49" s="1">
         <v>0.28366202000000001</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E49" s="2">
         <v>5.9999999999999997E-7</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A50" s="1">
         <v>-4</v>
       </c>
-      <c r="B49">
+      <c r="B50" s="1">
         <v>-0.65364359999999999</v>
       </c>
-      <c r="C49">
+      <c r="C50" s="1">
         <v>16</v>
       </c>
-      <c r="D49">
+      <c r="D50" s="1">
         <v>-0.65364359999999999</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E50" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A51" s="1">
         <v>-3</v>
       </c>
-      <c r="B50">
+      <c r="B51" s="1">
         <v>-0.98999250000000005</v>
       </c>
-      <c r="C50">
+      <c r="C51" s="1">
         <v>16</v>
       </c>
-      <c r="D50">
+      <c r="D51" s="1">
         <v>-0.9899926</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E51" s="2">
         <v>9.9999999999999995E-8</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A52" s="1">
         <v>-2</v>
       </c>
-      <c r="B51">
+      <c r="B52" s="1">
         <v>-0.41614684000000002</v>
       </c>
-      <c r="C51">
+      <c r="C52" s="1">
         <v>16</v>
       </c>
-      <c r="D51">
+      <c r="D52" s="1">
         <v>-0.41614676</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E52" s="2">
         <v>1.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A53" s="1">
         <v>-1</v>
       </c>
-      <c r="B52">
+      <c r="B53" s="1">
         <v>0.54030230000000001</v>
       </c>
-      <c r="C52">
+      <c r="C53" s="1">
         <v>16</v>
       </c>
-      <c r="D52">
+      <c r="D53" s="1">
         <v>0.54030230000000001</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E53" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A54" s="1">
         <v>0</v>
       </c>
-      <c r="B53">
+      <c r="B54" s="1">
         <v>1</v>
       </c>
-      <c r="C53">
+      <c r="C54" s="1">
         <v>16</v>
       </c>
-      <c r="D53">
+      <c r="D54" s="1">
         <v>1</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E54" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A55" s="1">
         <v>1</v>
       </c>
-      <c r="B54">
+      <c r="B55" s="1">
         <v>0.54030230000000001</v>
       </c>
-      <c r="C54">
+      <c r="C55" s="1">
         <v>16</v>
       </c>
-      <c r="D54">
+      <c r="D55" s="1">
         <v>0.54030230000000001</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E55" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A56" s="1">
         <v>2</v>
       </c>
-      <c r="B55">
+      <c r="B56" s="1">
         <v>-0.41614684000000002</v>
       </c>
-      <c r="C55">
+      <c r="C56" s="1">
         <v>16</v>
       </c>
-      <c r="D55">
+      <c r="D56" s="1">
         <v>-0.41614676</v>
       </c>
-      <c r="E55" s="1">
+      <c r="E56" s="2">
         <v>1.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56">
-        <v>3</v>
-      </c>
-      <c r="B56">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A57" s="1">
+        <v>3</v>
+      </c>
+      <c r="B57" s="1">
         <v>-0.98999250000000005</v>
       </c>
-      <c r="C56">
+      <c r="C57" s="1">
         <v>16</v>
       </c>
-      <c r="D56">
+      <c r="D57" s="1">
         <v>-0.9899926</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E57" s="2">
         <v>9.9999999999999995E-8</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A58" s="1">
         <v>4</v>
       </c>
-      <c r="B57">
+      <c r="B58" s="1">
         <v>-0.65364359999999999</v>
       </c>
-      <c r="C57">
+      <c r="C58" s="1">
         <v>16</v>
       </c>
-      <c r="D57">
+      <c r="D58" s="1">
         <v>-0.65364359999999999</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E58" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A59" s="1">
         <v>5</v>
       </c>
-      <c r="B58">
+      <c r="B59" s="1">
         <v>0.28366219999999998</v>
       </c>
-      <c r="C58">
+      <c r="C59" s="1">
         <v>16</v>
       </c>
-      <c r="D58">
+      <c r="D59" s="1">
         <v>0.28366202000000001</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E59" s="2">
         <v>5.9999999999999997E-7</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A60" s="1">
         <v>6</v>
       </c>
-      <c r="B59">
+      <c r="B60" s="1">
         <v>0.96017026999999999</v>
       </c>
-      <c r="C59">
+      <c r="C60" s="1">
         <v>16</v>
       </c>
-      <c r="D59">
+      <c r="D60" s="1">
         <v>0.96017019999999997</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E60" s="2">
         <v>9.9999999999999995E-8</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A61" s="1">
         <v>7</v>
       </c>
-      <c r="B60">
+      <c r="B61" s="1">
         <v>0.75390226000000005</v>
       </c>
-      <c r="C60">
+      <c r="C61" s="1">
         <v>16</v>
       </c>
-      <c r="D60">
+      <c r="D61" s="1">
         <v>0.75390239999999997</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E61" s="2">
         <v>1.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A62" s="1">
         <v>8</v>
       </c>
-      <c r="B61">
+      <c r="B62" s="1">
         <v>-0.14550003</v>
       </c>
-      <c r="C61">
+      <c r="C62" s="1">
         <v>16</v>
       </c>
-      <c r="D61">
+      <c r="D62" s="1">
         <v>-0.14549993999999999</v>
       </c>
-      <c r="E61" s="1">
+      <c r="E62" s="2">
         <v>5.9999999999999997E-7</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A62">
-        <v>9</v>
-      </c>
-      <c r="B62">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A63" s="1">
+        <v>9</v>
+      </c>
+      <c r="B63" s="1">
         <v>-0.91113025000000003</v>
       </c>
-      <c r="C62">
+      <c r="C63" s="1">
         <v>16</v>
       </c>
-      <c r="D62">
+      <c r="D63" s="1">
         <v>-0.91113010000000005</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E63" s="2">
         <v>1.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A63">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A64" s="1">
         <v>10</v>
       </c>
-      <c r="B63">
+      <c r="B64" s="1">
         <v>-0.83907149999999997</v>
       </c>
-      <c r="C63">
+      <c r="C64" s="1">
         <v>16</v>
       </c>
-      <c r="D63">
+      <c r="D64" s="1">
         <v>-0.83907175000000001</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E64" s="2">
         <v>2.9999999999999999E-7</v>
       </c>
     </row>

</xml_diff>